<commit_message>
First run of Spreadsheet processing script. Next steps for this script are:     Drop "contrasts" from the subset tables object before writing to     spreadsheets
    Add biologically significant tables to spreadsheets

 Changes to be committed:
	modified:   Pax6Epi_PCO_Write_Excel.R
	new file:   analysis_results/WTLEvP6LE_DBI_WT_24_Hour.xlsx
	new file:   analysis_results/WTLEvP6LE_DBI_WT_48_Hour.xlsx
	new file:   analysis_results/WTLEvP6LE_DNA_WT_24_Hour.xlsx
	new file:   analysis_results/WTLEvP6LE_DNA_WT_6_Hour.xlsx
	modified:   data_files/Comparisons.xlsx
</commit_message>
<xml_diff>
--- a/data_files/Comparisons.xlsx
+++ b/data_files/Comparisons.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="86">
   <si>
     <t xml:space="preserve">Analysis Overview  --  Overlap between Pax6  dependent genes, and genes differentially regulated in PCO model at &lt;6,24,24 Hours&gt; </t>
   </si>
@@ -249,15 +249,6 @@
     <t xml:space="preserve">The fold change of this gene between WT and FN at Zero Hours</t>
   </si>
   <si>
-    <t xml:space="preserve">5 (E)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logFC_WT_0_Hour_vs_FN_0_Hour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Log (base 2) of the fold change of this gene between WT and FN at Zero Hours</t>
-  </si>
-  <si>
     <t xml:space="preserve">6 (F)</t>
   </si>
   <si>
@@ -292,15 +283,6 @@
   </si>
   <si>
     <t xml:space="preserve">The fold change of this gene between WT and FN at 24 Hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 (J)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logFC_WT_48_Hour_vs_FN_48_Hour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Log (base 2) of the fold change of this gene between WT and FN at 24 Hours</t>
   </si>
   <si>
     <t xml:space="preserve">11 (K)</t>
@@ -537,10 +519,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:F64"/>
+  <dimension ref="B1:F62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C57" activeCellId="0" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1086,10 +1068,10 @@
         <v>66</v>
       </c>
       <c r="D55" s="6"/>
-      <c r="E55" s="6" t="s">
+      <c r="E55" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="F55" s="6"/>
+      <c r="F55" s="17"/>
     </row>
     <row r="56" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="16" t="s">
@@ -1099,10 +1081,10 @@
         <v>69</v>
       </c>
       <c r="D56" s="6"/>
-      <c r="E56" s="17" t="s">
+      <c r="E56" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F56" s="17"/>
+      <c r="F56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="16" t="s">
@@ -1138,10 +1120,10 @@
         <v>78</v>
       </c>
       <c r="D59" s="6"/>
-      <c r="E59" s="6" t="s">
+      <c r="E59" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="F59" s="6"/>
+      <c r="F59" s="17"/>
     </row>
     <row r="60" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="16" t="s">
@@ -1164,45 +1146,19 @@
         <v>84</v>
       </c>
       <c r="D61" s="6"/>
-      <c r="E61" s="17" t="s">
+      <c r="E61" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F61" s="17"/>
-    </row>
-    <row r="62" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B62" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F62" s="6"/>
-    </row>
-    <row r="63" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B63" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F63" s="6"/>
-    </row>
+      <c r="F61" s="6"/>
+    </row>
+    <row r="62" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="64" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="65" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="66" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="67" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="44">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F8"/>
     <mergeCell ref="B9:F9"/>
@@ -1247,10 +1203,6 @@
     <mergeCell ref="E60:F60"/>
     <mergeCell ref="C61:D61"/>
     <mergeCell ref="E61:F61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="E63:F63"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Finalized R Scripts in Pipeline, Updated README.md
</commit_message>
<xml_diff>
--- a/data_files/Comparisons.xlsx
+++ b/data_files/Comparisons.xlsx
@@ -20,13 +20,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
   <si>
     <t xml:space="preserve">Analysis Overview  --  Overlap between Pax6  dependent genes, and genes differentially regulated in PCO model at &lt;6,24,24 Hours&gt; </t>
   </si>
   <si>
-    <t xml:space="preserve">Integrated analysis comparing genes differentially expressed in lens epithelial cells from wild type and Pax6 null mice to genes differentially expressed in a mouse model of cataract surgery at &lt;6,24,48&gt; hours. Comparisons in this data set are made between two separate pairwise contrasts, designated WTvP6 and WT0vWT6,24,48.  Genes differentially expressed at 0 hours are identified in contrast WT0vFN0.   Genes differentially expressed at 24 Hours are identified in contrast WT0vWT24.  In both contrasts, positive fold changes are associated with increased expression in Fibronectin conditional knockouts (FN) over wildtype (WT).  
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Integrated analysis comparing genes differentially expressed in lens epithelial cells from wild type and Pax6 null mice to genes differentially expressed in a mouse model of cataract surgery at &lt;6,24,48&gt; hours. Comparisons in this data set are made between two separate pairwise contrasts, designated WTvP6 and WT0vWT6,24,48.  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Differential gene expression</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in lens epithelial cells between Pax6 heterozygous mice and their wildtype litter mates is measured in the contrast WTvP6.  Differential gene expression in cells isolated from lens capsular bags between zero and  24 hours post surgery is measured in the contrast WT0vWT24.  In the contrast WTvP6, positive fold changes are associated with increased expression in Pax6 heterozygotes over wildtype (WT).  In the contrast WT0vWT24, positive fold changes are associated with increased expression at 24 hours over zero hours
 Reviewed by:</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Worksheet Specification</t>
@@ -50,13 +78,13 @@
     <t xml:space="preserve">All genes common to both pairwise contrasts differentially expressed with an absolute fold change &gt; 2 and an FDR less than 0.05</t>
   </si>
   <si>
-    <t xml:space="preserve">SS Down WTvP6 Up WT0vWT24</t>
+    <t xml:space="preserve">SS Dn WTvP6 Up WT0vWT24</t>
   </si>
   <si>
     <t xml:space="preserve">Statistically significant genes, decreased expression in Pax6 Heterozygotes over Wildtype, increased expression at 24 Hours over 0 Hours</t>
   </si>
   <si>
-    <t xml:space="preserve">SS Down WTvP6 Down WT0vWT24</t>
+    <t xml:space="preserve">SS Dn WTvP6 Dn WT0vWT24</t>
   </si>
   <si>
     <t xml:space="preserve">Statistically significant genes, decreased expression Pax6 Heterozygotes over Wildtype, decreased expression at 24 Hours over 0 Hours</t>
@@ -68,7 +96,7 @@
     <t xml:space="preserve">Statistically significant genes, increased expression Pax6 Heterozygotes over Wildtype, increased expression at 24 Hours over 0 Hours</t>
   </si>
   <si>
-    <t xml:space="preserve">SS Up WTvP6 Down WT0vWT24</t>
+    <t xml:space="preserve">SS Up WTvP6 Dn WT0vWT24</t>
   </si>
   <si>
     <t xml:space="preserve">Statistically significant genes, increased expression Pax6 Heterozygotes over Wildtype, decreased expression at 24 Hours over 0 Hours</t>
@@ -80,12 +108,15 @@
     <t xml:space="preserve">All genes common to both pairwise contrasts meeting criteria for biologically significant differential expression</t>
   </si>
   <si>
-    <t xml:space="preserve">BS Down WTvP6 Up WT0vWT24</t>
+    <t xml:space="preserve">BS Dn WTvP6 Up WT0vWT24</t>
   </si>
   <si>
     <t xml:space="preserve">Biologically significant genes, decreased expression Pax6 Heterozygotes over Wildtype, increased expression at 24 Hours over 0 Hours</t>
   </si>
   <si>
+    <t xml:space="preserve">BS Dn WTvP6 Dn WT0vWT24</t>
+  </si>
+  <si>
     <t xml:space="preserve">Biologically significant genes, decreased expression Pax6 Heterozygotes over Wildtype, decreased expression at 24 Hours over 0 Hours</t>
   </si>
   <si>
@@ -93,6 +124,9 @@
   </si>
   <si>
     <t xml:space="preserve">Biologically significant genes, increased expression Pax6 Heterozygotes over Wildtype, increased expression at 24 Hours over 0 Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS Up WTvP6 Dn WT0vWT24</t>
   </si>
   <si>
     <t xml:space="preserve">Biologically significant genes, increased expression Pax6 Heterozygotes over Wildtype, decreased expression at 24 Hours over 0 Hours</t>
@@ -165,10 +199,10 @@
     <t xml:space="preserve">Total</t>
   </si>
   <si>
-    <t xml:space="preserve">Upregulated (FncKO)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Downregulated (FncKO)</t>
+    <t xml:space="preserve">Upregulated (Pax6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Downregulated (Pax6)</t>
   </si>
   <si>
     <t xml:space="preserve">Statistically Significant</t>
@@ -180,25 +214,25 @@
     <t xml:space="preserve">Genes Differentially Regulated Between Zero and &lt;6, 24, 48&gt; Hours</t>
   </si>
   <si>
-    <t xml:space="preserve">Upregulated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Downregulated</t>
+    <t xml:space="preserve">Upregulated (24 Hours)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Downregulated (24 Hours)</t>
   </si>
   <si>
     <t xml:space="preserve">Statistically Significant Intersection</t>
   </si>
   <si>
-    <t xml:space="preserve">Up 24 Hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Down 24 Hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Up 0 Hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Down 0 Hours</t>
+    <t xml:space="preserve">Up Pax6 Het.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Down Pax6 Het.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Up WT_24_Hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Down WT_24_Hour</t>
   </si>
   <si>
     <t xml:space="preserve">Biologically Significant Intersection</t>
@@ -216,7 +250,7 @@
     <t xml:space="preserve">1 (A)</t>
   </si>
   <si>
-    <t xml:space="preserve">GeneID</t>
+    <t xml:space="preserve">MGI.symbol</t>
   </si>
   <si>
     <t xml:space="preserve">The symbol used to identify this gene</t>
@@ -243,73 +277,73 @@
     <t xml:space="preserve">4 (D)</t>
   </si>
   <si>
-    <t xml:space="preserve">FC_WT_0_Hour_vs_FN_0_Hour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The fold change of this gene between WT and FN at Zero Hours</t>
+    <t xml:space="preserve">Pax6_LE_Fold_Change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The fold change of this gene between WT and P6</t>
   </si>
   <si>
     <t xml:space="preserve">6 (F)</t>
   </si>
   <si>
-    <t xml:space="preserve">FDR_WT_0_Hour_vs_FN_0_Hour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benjamini Hochburg adjusted P value returned by edgeR's topTags function (WT vs FN at 0 hours)</t>
+    <t xml:space="preserve">Pax6_LE_FDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_Value calculated by Cuffdiff (WT vs P6)</t>
   </si>
   <si>
     <t xml:space="preserve">7 (G)</t>
   </si>
   <si>
-    <t xml:space="preserve">WT_0_Hour_Avg_RPKM.g1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abundance of this gene (Average RPKM) observed in WT at zero hours</t>
+    <t xml:space="preserve">Pax6_LE_plusplus_Avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abundance of this gene (Average FPKM) observed in WT Lens Epithelia</t>
   </si>
   <si>
     <t xml:space="preserve">8 (H)</t>
   </si>
   <si>
-    <t xml:space="preserve">FN_0_Hour_Avg_RPKM.g1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abundance of this gene (Average RPKM) observed in FN at zero hours</t>
+    <t xml:space="preserve">Pax6_LE_plusminus_Avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abundance of this gene (Average FPKM) observed in Pax6 Heterozygous (Het) Lens Epithelia</t>
   </si>
   <si>
     <t xml:space="preserve">9 (I)</t>
   </si>
   <si>
-    <t xml:space="preserve">FC_WT_48_Hour_vs_FN_48_Hour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The fold change of this gene between WT and FN at 24 Hours</t>
+    <t xml:space="preserve">WT0vWT24_Fold_Change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The fold change of this gene between zero and 24 Hours in WT</t>
   </si>
   <si>
     <t xml:space="preserve">11 (K)</t>
   </si>
   <si>
-    <t xml:space="preserve">FDR_WT_48_Hour_vs_FN_48_Hour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benjamini Hochburg adjusted P value returned by edgeR's topTags function (WT vs FN at 24 Hours)</t>
+    <t xml:space="preserve">WT0vWT24_FDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benjamini Hochburg adjusted P value returned by edgeR's topTags function (zero vs 24 Hours)</t>
   </si>
   <si>
     <t xml:space="preserve">12 (L)</t>
   </si>
   <si>
-    <t xml:space="preserve">WT_48_Hour_Avg_RPKM.g2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abundance of this gene (Average RPKM) observed in WT at 24 Hours</t>
+    <t xml:space="preserve">WT0vWT24_WT_0_Hour_Avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abundance of this gene (Average F/RPKM) observed in WT at 0 Hours</t>
   </si>
   <si>
     <t xml:space="preserve">13 (M)</t>
   </si>
   <si>
-    <t xml:space="preserve">FN_48_Hour_Avg_RPKM.g2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abundance of this gene (Average RPKM) observed in FN at 24 Hours</t>
+    <t xml:space="preserve">WT0vWT24_WT_24_Hour_Avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abundance of this gene (Average F/RPKM) observed in WT at 24 Hours</t>
   </si>
 </sst>
 </file>
@@ -319,7 +353,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -356,6 +390,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -482,7 +522,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -521,17 +561,18 @@
   </sheetPr>
   <dimension ref="B1:F62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C57" activeCellId="0" sqref="C57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="73.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="70.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.57"/>
   </cols>
   <sheetData>
@@ -705,10 +746,10 @@
     </row>
     <row r="19" customFormat="false" ht="17.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -716,10 +757,10 @@
     </row>
     <row r="20" customFormat="false" ht="17.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -727,10 +768,10 @@
     </row>
     <row r="21" customFormat="false" ht="17.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -744,7 +785,7 @@
     </row>
     <row r="23" customFormat="false" ht="31.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -753,45 +794,45 @@
     </row>
     <row r="24" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F27" s="3"/>
     </row>
@@ -810,7 +851,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -819,22 +860,22 @@
     </row>
     <row r="31" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
@@ -843,7 +884,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
@@ -859,7 +900,7 @@
     </row>
     <row r="35" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -868,22 +909,22 @@
     </row>
     <row r="36" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
@@ -892,7 +933,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
@@ -913,20 +954,20 @@
     </row>
     <row r="41" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E41" s="12"/>
       <c r="F41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="14" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
@@ -935,7 +976,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
@@ -951,20 +992,20 @@
     </row>
     <row r="45" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E45" s="12"/>
       <c r="F45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="14" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
@@ -973,7 +1014,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
@@ -988,7 +1029,7 @@
     </row>
     <row r="49" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -997,10 +1038,10 @@
     </row>
     <row r="50" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="8" t="s">
@@ -1010,144 +1051,144 @@
     </row>
     <row r="51" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F52" s="6"/>
     </row>
     <row r="53" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F55" s="17"/>
     </row>
     <row r="56" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="16" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F59" s="17"/>
     </row>
     <row r="60" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="16" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F61" s="6"/>
     </row>

</xml_diff>